<commit_message>
removed the *2 from the login names
</commit_message>
<xml_diff>
--- a/resources/SampleData.xlsx
+++ b/resources/SampleData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="11760" windowHeight="4365"/>
+    <workbookView windowWidth="8745" windowHeight="3315"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,10 +104,10 @@
   <numFmts count="6">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="9" formatCode="0%"/>
-    <numFmt numFmtId="602" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="603" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="604" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="605" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="774" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="775" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="776" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="777" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -193,10 +193,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="604" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="602" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="605" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="603" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="776" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="774" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="777" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="775" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="1" applyFont="1" applyFill="1"/>

</xml_diff>

<commit_message>
minor changes to excel
</commit_message>
<xml_diff>
--- a/resources/SampleData.xlsx
+++ b/resources/SampleData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="8745" windowHeight="3315"/>
+    <workbookView windowWidth="2250" windowHeight="2250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,10 +104,10 @@
   <numFmts count="6">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="9" formatCode="0%"/>
-    <numFmt numFmtId="774" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="775" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="776" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="777" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="946" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="947" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="948" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="949" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -193,10 +193,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="776" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="774" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="777" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="775" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="948" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="946" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="949" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="947" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="1" applyFont="1" applyFill="1"/>

</xml_diff>

<commit_message>
changed the data file
</commit_message>
<xml_diff>
--- a/resources/SampleData.xlsx
+++ b/resources/SampleData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="2250" windowHeight="2250"/>
+    <workbookView windowWidth="7710" windowHeight="3540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>LastName</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Ford</t>
   </si>
   <si>
-    <t>Pford</t>
+    <t>Pford1</t>
   </si>
   <si>
     <t>pford@aos.com</t>
@@ -52,7 +52,7 @@
     <t>Arthur</t>
   </si>
   <si>
-    <t>arthur</t>
+    <t>arthur1</t>
   </si>
   <si>
     <t>arthur@aos.com</t>
@@ -67,6 +67,9 @@
     <t>Zaphod</t>
   </si>
   <si>
+    <t>Zaphod1</t>
+  </si>
+  <si>
     <t>zaph@aos.com</t>
   </si>
   <si>
@@ -79,7 +82,7 @@
     <t>Dirk</t>
   </si>
   <si>
-    <t>Gdirk</t>
+    <t>Gdirk1</t>
   </si>
   <si>
     <t>dirk@aos.com</t>
@@ -89,6 +92,9 @@
   </si>
   <si>
     <t>Trillian</t>
+  </si>
+  <si>
+    <t>Trillian1</t>
   </si>
   <si>
     <t>trilli@aos.com</t>
@@ -104,10 +110,10 @@
   <numFmts count="6">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="9" formatCode="0%"/>
-    <numFmt numFmtId="946" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="947" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="948" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="949" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="1376" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="1377" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="1378" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="1379" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -193,10 +199,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="948" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="946" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="949" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="947" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="1378" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="1376" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="1379" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="1377" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="1" applyFont="1" applyFill="1"/>
@@ -285,47 +291,47 @@
         <v>16</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>